<commit_message>
added support for multiple elective options
</commit_message>
<xml_diff>
--- a/example_input.xlsx
+++ b/example_input.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>slot 1</t>
   </si>
@@ -62,6 +62,12 @@
     <t>algebra 2</t>
   </si>
   <si>
+    <t>psy</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
     <t>/</t>
   </si>
   <si>
@@ -84,6 +90,12 @@
   </si>
   <si>
     <t>elective</t>
+  </si>
+  <si>
+    <t>elective2</t>
+  </si>
+  <si>
+    <t>elective3</t>
   </si>
   <si>
     <t>alice</t>
@@ -102,8 +114,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -114,41 +126,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -160,6 +142,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -168,23 +158,96 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -192,58 +255,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -251,8 +262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,55 +279,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,127 +453,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,17 +482,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,15 +538,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -535,17 +547,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,8 +565,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,148 +575,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1034,7 +1046,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="6"/>
@@ -1090,17 +1102,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1112,43 +1136,49 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1171,10 +1201,16 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1196,11 +1232,14 @@
       </c>
       <c r="H3" t="s">
         <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>

</xml_diff>